<commit_message>
Commit 2 with BDD codes
</commit_message>
<xml_diff>
--- a/RestAssuredMaven/Data/Postdata.xlsx
+++ b/RestAssuredMaven/Data/Postdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11310" windowHeight="2250"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,49 +33,49 @@
     <t>Email</t>
   </si>
   <si>
-    <t>FNA4</t>
-  </si>
-  <si>
-    <t>LNA4</t>
-  </si>
-  <si>
-    <t>UNA4</t>
-  </si>
-  <si>
-    <t>PSA4</t>
-  </si>
-  <si>
-    <t>EMA4</t>
-  </si>
-  <si>
-    <t>FNA5</t>
-  </si>
-  <si>
-    <t>LNA5</t>
-  </si>
-  <si>
-    <t>UNA5</t>
-  </si>
-  <si>
-    <t>PSA5</t>
-  </si>
-  <si>
-    <t>EMA5</t>
-  </si>
-  <si>
-    <t>FNA6</t>
-  </si>
-  <si>
-    <t>LNA6</t>
-  </si>
-  <si>
-    <t>UNA6</t>
-  </si>
-  <si>
-    <t>PSA6</t>
-  </si>
-  <si>
-    <t>EMA6</t>
+    <t>FNC7</t>
+  </si>
+  <si>
+    <t>FNC8</t>
+  </si>
+  <si>
+    <t>FNC9</t>
+  </si>
+  <si>
+    <t>LNC7</t>
+  </si>
+  <si>
+    <t>LNC8</t>
+  </si>
+  <si>
+    <t>LNC9</t>
+  </si>
+  <si>
+    <t>UNC7</t>
+  </si>
+  <si>
+    <t>UNC8</t>
+  </si>
+  <si>
+    <t>UNC9</t>
+  </si>
+  <si>
+    <t>PSC7</t>
+  </si>
+  <si>
+    <t>PSC8</t>
+  </si>
+  <si>
+    <t>PSC9</t>
+  </si>
+  <si>
+    <t>EMC7</t>
+  </si>
+  <si>
+    <t>EMC8</t>
+  </si>
+  <si>
+    <t>EMC9</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -437,47 +437,47 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>

</xml_diff>